<commit_message>
update type class and typeService class
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenminhduy941gmail.com/Documents/Documents/java Full Stack/Hibernate_CuongNM_DuyNM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DFFD7F-9BB8-9E49-B538-0A8FE8510713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6A07D4-7020-8744-A256-9B6527571BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{4FEA7247-0345-6546-8294-C54F4C442E0A}"/>
   </bookViews>
@@ -925,7 +925,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,9 +946,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
create movie type dao
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenminhduy941gmail.com/Documents/Documents/java Full Stack/Hibernate_CuongNM_DuyNM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9E6B5D-0FF0-A84F-9995-95D58B0FB1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD708879-2F93-354A-93A6-FF15FAFA4C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{4FEA7247-0345-6546-8294-C54F4C442E0A}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="1" xr2:uid="{4FEA7247-0345-6546-8294-C54F4C442E0A}"/>
   </bookViews>
   <sheets>
     <sheet name="TYPE" sheetId="1" r:id="rId1"/>
-    <sheet name="MOVIE_TYPE" sheetId="3" r:id="rId2"/>
-    <sheet name="MOVIE" sheetId="4" r:id="rId3"/>
+    <sheet name="MOVIE" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Decription</t>
   </si>
   <si>
-    <t>Very good</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -87,12 +83,6 @@
   </si>
   <si>
     <t>small_image</t>
-  </si>
-  <si>
-    <t>ID_TYPE</t>
-  </si>
-  <si>
-    <t>ID_MOVIE</t>
   </si>
   <si>
     <t>lotte</t>
@@ -190,82 +180,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <strike val="0"/>
@@ -580,30 +495,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BACD4DAD-7D01-E948-B036-26DBA9F56DC2}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BACD4DAD-7D01-E948-B036-26DBA9F56DC2}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:C2" xr:uid="{BACD4DAD-7D01-E948-B036-26DBA9F56DC2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{192344F7-7C88-784E-A410-6E78A6753E84}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{4CA4AB72-74C0-C74B-8D0A-59D68481FFB7}" name="Name" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{4EE89306-68D2-5C49-BFA8-C6B828325D8A}" name="Decription" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{192344F7-7C88-784E-A410-6E78A6753E84}" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{4CA4AB72-74C0-C74B-8D0A-59D68481FFB7}" name="Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{4EE89306-68D2-5C49-BFA8-C6B828325D8A}" name="Decription" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4EF0E58-3BCF-6C4A-854F-F366BACAF1A9}" name="Table4" displayName="Table4" ref="A1:C2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:C2" xr:uid="{F4EF0E58-3BCF-6C4A-854F-F366BACAF1A9}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E165CED6-935D-044A-85C7-F0D1408CCA73}" name="ID_TYPE" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{2A5D7725-E879-ED4F-853E-37E266F2EB09}" name="ID_MOVIE" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{C540009C-284F-A341-8489-EA223F8E692E}" name="Decription" dataDxfId="15"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D148110B-F30E-7C41-8395-AD2210FF9C18}" name="Table33" displayName="Table33" ref="A1:M2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M2" xr:uid="{D148110B-F30E-7C41-8395-AD2210FF9C18}"/>
   <tableColumns count="13">
@@ -924,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB316C93-902B-2845-BC4E-0F3D3CB10AD1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -950,7 +853,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
         <v>20</v>
@@ -965,57 +868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED14AC5-3BAE-8349-B382-B0E74A458D85}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C4A57A-CD5E-834D-9AA3-BCF9CB47B8E5}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,40 +895,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="26" x14ac:dyDescent="0.3">
@@ -1079,10 +936,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">

</xml_diff>